<commit_message>
Improvising test dats sheet
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Crestech\Appium\CrestechMobileTesting\CrestechMobileTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE883E5-67E8-4E4B-B64B-5D80CACA5AB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B0AB62-14E7-452C-9D9B-AA4F127DF91A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -67,12 +67,6 @@
     <t>pCloudyIOS</t>
   </si>
   <si>
-    <t>deviceName</t>
-  </si>
-  <si>
-    <t>platformVersion</t>
-  </si>
-  <si>
     <t>pCloudy_Username</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t>pCloudy_DurationInMinutes</t>
   </si>
   <si>
-    <t>pCloudy_DeviceFullName</t>
-  </si>
-  <si>
     <t>bundleId</t>
   </si>
   <si>
@@ -100,12 +91,6 @@
     <t>Safari</t>
   </si>
   <si>
-    <t>11.2</t>
-  </si>
-  <si>
-    <t>iPhone 6</t>
-  </si>
-  <si>
     <t>46939d639fe3d4da0cb33e172f2c27701dfa1e9f</t>
   </si>
   <si>
@@ -136,12 +121,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>Redmi 6 Pro</t>
-  </si>
-  <si>
-    <t>9.0.0</t>
-  </si>
-  <si>
     <t>com.example.android.apis.ApiDemos</t>
   </si>
   <si>
@@ -233,9 +212,6 @@
   </si>
   <si>
     <t>Syska Smart Home.apk</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyS8_Android_8.0.0</t>
   </si>
 </sst>
 </file>
@@ -298,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
@@ -309,7 +285,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
@@ -650,77 +625,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="14.7109375" style="3"/>
+    <col min="2" max="2" width="45.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="14.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>16</v>
@@ -728,39 +701,34 @@
       <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="D2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>5</v>
@@ -768,58 +736,49 @@
       <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>5</v>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>5</v>
@@ -842,163 +801,133 @@
       <c r="P3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>5</v>
@@ -1006,85 +935,67 @@
       <c r="L7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>61</v>
+      <c r="P8" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1105,44 +1016,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>68</v>
+        <v>49</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1163,7 +1074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1171,23 +1082,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Modified application method with alert handling Signed-off-by: Admin <Admin@CTNL0034.crestechad.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitAutomation\DBS_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -164,12 +164,6 @@
     <t>com.pcloudy.appiumdemo</t>
   </si>
   <si>
-    <t>sakshi.juneja@crestechsoftware.com</t>
-  </si>
-  <si>
-    <t>t68k6kw68ywjv2y9zwfr9r3t</t>
-  </si>
-  <si>
     <t>pCloudy_Appium_Demo.apk</t>
   </si>
   <si>
@@ -188,31 +182,37 @@
     <t>divya.devi@crestechsoftware.com</t>
   </si>
   <si>
-    <t>testmunk</t>
-  </si>
-  <si>
-    <t>test@testname.com</t>
-  </si>
-  <si>
-    <t>test123@testname.com</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone7plus_iOS_13.5.1_b1cc7</t>
-  </si>
-  <si>
-    <t>13.5.1</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone8plus_iOS_14.3.0_a0940</t>
-  </si>
-  <si>
-    <t>14.3.0</t>
-  </si>
-  <si>
     <t>TestmunkDemo_Resigned1634793440.ipa</t>
   </si>
   <si>
     <t>r36d4py9mtkykt29c925c7mg</t>
+  </si>
+  <si>
+    <t>ONEPLUS_9_Android_11.0.0_a5ac6</t>
+  </si>
+  <si>
+    <t>11.0.0</t>
+  </si>
+  <si>
+    <t>S7762772C</t>
+  </si>
+  <si>
+    <t>224433</t>
+  </si>
+  <si>
+    <t>shubham.gupta@crestechsoftware.com</t>
+  </si>
+  <si>
+    <t>9jyrcnpjj7y2353rybtv8n49</t>
+  </si>
+  <si>
+    <t>com.dbs.sg.digibank.ui.demo.SplashActivity</t>
+  </si>
+  <si>
+    <t>com.dbs.sit1.dbsmbanking</t>
+  </si>
+  <si>
+    <t>dbsandroidUAT_10Nov.apk</t>
   </si>
 </sst>
 </file>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,6 +349,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -657,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +749,7 @@
         <v>46</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>41</v>
@@ -752,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>5</v>
@@ -776,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>5</v>
@@ -878,15 +884,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>46</v>
+      <c r="B6" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -916,16 +922,16 @@
         <v>5</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="N6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -936,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>5</v>
@@ -966,13 +972,13 @@
         <v>5</v>
       </c>
       <c r="M7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="O7" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>37</v>
@@ -1039,72 +1045,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code modification at the run trigger time Signed-off-by: Admin <Admin@CTNL0034.crestechad.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -188,18 +188,9 @@
     <t>r36d4py9mtkykt29c925c7mg</t>
   </si>
   <si>
-    <t>ONEPLUS_9_Android_11.0.0_a5ac6</t>
-  </si>
-  <si>
     <t>11.0.0</t>
   </si>
   <si>
-    <t>S7762772C</t>
-  </si>
-  <si>
-    <t>224433</t>
-  </si>
-  <si>
     <t>shubham.gupta@crestechsoftware.com</t>
   </si>
   <si>
@@ -213,13 +204,37 @@
   </si>
   <si>
     <t>dbsandroidUAT_10Nov.apk</t>
+  </si>
+  <si>
+    <t>Manafacturer</t>
+  </si>
+  <si>
+    <t>Min_Ver</t>
+  </si>
+  <si>
+    <t>Max_Ver</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
+  </si>
+  <si>
+    <t>Individual_ID</t>
+  </si>
+  <si>
+    <t>S7768075F</t>
+  </si>
+  <si>
+    <t>909760</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,19 +270,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -295,9 +308,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -340,14 +353,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -355,6 +361,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -663,11 +679,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.140625" style="6" bestFit="1" customWidth="1"/>
@@ -688,7 +704,7 @@
     <col min="17" max="16384" width="14.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -738,7 +754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -788,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -838,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -858,7 +874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -884,15 +900,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>62</v>
+      <c r="B6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -922,19 +938,19 @@
         <v>5</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="O6" s="21" t="s">
-        <v>63</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="11" customFormat="1">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -971,7 +987,7 @@
       <c r="L7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="16" t="s">
         <v>52</v>
       </c>
       <c r="N7" s="9" t="s">
@@ -984,7 +1000,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -1045,57 +1061,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>58</v>
-      </c>
+      <c r="B5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1111,7 +1183,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Wait changes -- implicit
Signed-off-by: Sakshi <sakshi.juneja@crestechsoftware.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DBS_NEW_WORKSPACE\DBS_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CFF65D-7DA5-43EA-9ED5-3E472B81F046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="101">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -206,35 +207,131 @@
     <t>Individual_ID</t>
   </si>
   <si>
-    <t>DBS_Android.apk</t>
-  </si>
-  <si>
     <t>12.0.0</t>
   </si>
   <si>
     <t>Xiaomi</t>
   </si>
   <si>
-    <t>S2325489AUID</t>
-  </si>
-  <si>
     <t>121212</t>
   </si>
   <si>
-    <t>HUAWEI_P30Lite_Android_10.0.0_875f5</t>
-  </si>
-  <si>
     <t>AppName</t>
   </si>
   <si>
     <t>DBS</t>
+  </si>
+  <si>
+    <t>sakshi.juneja@crestechsoftware.com</t>
+  </si>
+  <si>
+    <t>t68k6kw68ywjv2y9zwfr9r3t</t>
+  </si>
+  <si>
+    <t>dbsandroidUAT_10Nov.apk</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA10s_android_11.0.0_09401</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA12_android_11.0.0_334bc</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA21s_android_11.0.0_b13a4</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA31_android_11.0.0_32c0a</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA50_android_11.0.0_310bf</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA51_android_11.0.0_d52ba</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA71_android_11.0.0_fe4a3</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA9_android_10.0.0_6eed1</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyFold_android_9.0.0_d69de</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ4_android_10.0.0_889f0</t>
+  </si>
+  <si>
+    <t>11.0.0</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
+    <t>S2021218GUID</t>
+  </si>
+  <si>
+    <t>S2021219EUID</t>
+  </si>
+  <si>
+    <t>S2021220IUID</t>
+  </si>
+  <si>
+    <t>S2325474CUID</t>
+  </si>
+  <si>
+    <t>S2325475AUID</t>
+  </si>
+  <si>
+    <t>S2325476ZUID</t>
+  </si>
+  <si>
+    <t>S2325477HUID</t>
+  </si>
+  <si>
+    <t>S2325478FUID</t>
+  </si>
+  <si>
+    <t>S2325479DUID</t>
+  </si>
+  <si>
+    <t>S2325480HUID</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ6_android_10.0.0_482da</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ7Pro_android_9.0.0_a715a</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ7Pro_android_8.1.0_42e4e</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ8_android_10.0.0_882d2</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyM01_android_11.0.0_7425f</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyM02_android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyM10_android_10.0.0_a58e4</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyM12_android_11.0.0_df6a7</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyM20_android_8.1.0_258bd</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyM40_android_11.0.0_efd9b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,17 +374,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -303,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -311,12 +397,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -358,25 +459,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,6 +568,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -506,6 +620,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -681,14 +812,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.140625" style="6" bestFit="1" customWidth="1"/>
@@ -709,7 +840,7 @@
     <col min="17" max="16384" width="14.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -759,7 +890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -809,7 +940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -859,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -879,7 +1010,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -905,14 +1036,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -942,20 +1073,20 @@
       <c r="L6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="16" t="s">
-        <v>51</v>
+      <c r="M6" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="11" customFormat="1">
+    <row r="7" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -992,7 +1123,7 @@
       <c r="L7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="15" t="s">
         <v>51</v>
       </c>
       <c r="N7" s="9" t="s">
@@ -1005,7 +1136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -1057,133 +1188,382 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1"/>
-    <hyperlink ref="M6" r:id="rId2"/>
+    <hyperlink ref="M7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
-    <col min="3" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="B1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="19"/>
-    </row>
-    <row r="6" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>1</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="C9" s="17">
+        <v>2</v>
+      </c>
+      <c r="D9" s="17">
+        <v>3</v>
+      </c>
+      <c r="E9" s="17">
+        <v>4</v>
+      </c>
+      <c r="F9" s="17">
+        <v>5</v>
+      </c>
+      <c r="G9" s="17">
+        <v>6</v>
+      </c>
+      <c r="H9" s="17">
+        <v>7</v>
+      </c>
+      <c r="I9" s="17">
+        <v>8</v>
+      </c>
+      <c r="J9" s="17">
+        <v>9</v>
+      </c>
+      <c r="K9" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1193,15 +1573,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Changes. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DBS_NEW_WORKSPACE\DBS_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BCF9AA-CD75-4D3A-9492-3B68C5ECAAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Test Data" sheetId="5" r:id="rId3"/>
     <sheet name="DeviceMasterSheet" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="113">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -156,15 +155,6 @@
     <t>t68k6kw68ywjv2y9zwfr9r3t</t>
   </si>
   <si>
-    <t>dbsandroidUAT_10Nov.apk</t>
-  </si>
-  <si>
-    <t>11.0.0</t>
-  </si>
-  <si>
-    <t>9.0.0</t>
-  </si>
-  <si>
     <t>S2021219EUID</t>
   </si>
   <si>
@@ -205,21 +195,6 @@
   </si>
   <si>
     <t>iWEALTH</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyS10_Android_10.0.0_e4d87</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyS20FE5G_Android_11.0.0_2ff2c</t>
-  </si>
-  <si>
-    <t>HUAWEI_Mate10_Android_10.0.0_2af65</t>
-  </si>
-  <si>
-    <t>GOOGLE_Pixel2XL_Android_10.0.0_b877c</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyS215G_Android_11.0.0_a4b35</t>
   </si>
   <si>
     <t>SGMBONEAPPMB.ipa</t>
@@ -313,12 +288,114 @@
   <si>
     <t>M4520239IUID</t>
   </si>
+  <si>
+    <t>APPLE_iPhoneX_iOS_13.5.1_5640f</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone12mini_iOS_14.7.1_eaf14</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone13Pro_iOS_15.2.0_2d8ea</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone11Pro_iOS_14.4.0_6ccce</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone11ProMax_iOS_14.4.2_de1da</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone12Pro_iOS_14.2.1_0d955</t>
+  </si>
+  <si>
+    <t>13.5.1</t>
+  </si>
+  <si>
+    <t>14.7.1</t>
+  </si>
+  <si>
+    <t>15.2.0</t>
+  </si>
+  <si>
+    <t>14.4.0</t>
+  </si>
+  <si>
+    <t>14.4.2</t>
+  </si>
+  <si>
+    <t>14.2.1</t>
+  </si>
+  <si>
+    <t>APPLE_iPhoneSE2020_iOS_13.6.1_4989f</t>
+  </si>
+  <si>
+    <t>APPLE_iPhoneXR_iOS_13.3.1_1cb9d</t>
+  </si>
+  <si>
+    <t>13.6.1</t>
+  </si>
+  <si>
+    <t>13.3.1</t>
+  </si>
+  <si>
+    <t>divya.devi@crestechsoftware.com</t>
+  </si>
+  <si>
+    <t>r36d4py9mtkykt29c925c7mg</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone11Pro_iOS_13.0.0_3f7e0</t>
+  </si>
+  <si>
+    <t>13.0.0</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone12_iOS_14.1.0_a050d</t>
+  </si>
+  <si>
+    <t>14.1.0</t>
+  </si>
+  <si>
+    <t>APPLE_iPhoneSE_iOS_14.6.0_9d61f</t>
+  </si>
+  <si>
+    <t>14.6.0</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone13mini_iOS_15.2.0_22426</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone13_iOS_15.0.0_ad341</t>
+  </si>
+  <si>
+    <t>15.0.0</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone13Pro_iOS_15.0.0_2d2ae</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone8_iOS_14.0.1_aa631</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone12ProMax_iOS_14.6.0_de280</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone8plus_iOS_14.6.0_5cd33</t>
+  </si>
+  <si>
+    <t>APPLE_iPhone7_iOS_14.4.0_589b8</t>
+  </si>
+  <si>
+    <t>14.0.1</t>
+  </si>
+  <si>
+    <t>dbs_android_UAT_7_10_003_532.apk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +431,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -382,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -424,11 +519,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -524,23 +629,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -576,23 +664,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -768,11 +839,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -889,8 +960,8 @@
       <c r="N2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>40</v>
+      <c r="O2" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>22</v>
@@ -934,13 +1005,13 @@
         <v>5</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>22</v>
@@ -953,101 +1024,294 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="14" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>60</v>
+      <c r="B1" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" t="s">
+        <v>74</v>
+      </c>
+      <c r="T4" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>35</v>
@@ -1061,8 +1325,53 @@
       <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1081,8 +1390,53 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1101,8 +1455,53 @@
       <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1121,8 +1520,53 @@
       <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1136,18 +1580,63 @@
         <v>3</v>
       </c>
       <c r="E9" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>5</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>5</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="11">
+        <v>1</v>
+      </c>
+      <c r="N9" s="11">
+        <v>5</v>
+      </c>
+      <c r="O9" s="11">
+        <v>1</v>
+      </c>
+      <c r="P9" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>1</v>
+      </c>
+      <c r="R9" s="11">
+        <v>1</v>
+      </c>
+      <c r="S9" s="11">
+        <v>5</v>
+      </c>
+      <c r="T9" s="11">
+        <v>1</v>
+      </c>
+      <c r="U9" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
@@ -1161,27 +1650,71 @@
       <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="13" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,72 +1804,72 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>72</v>
+      <c r="A2" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" t="s">
-        <v>51</v>
-      </c>
       <c r="L2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" t="s">
         <v>55</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" t="s">
         <v>63</v>
       </c>
-      <c r="N2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T2" t="s">
-        <v>70</v>
-      </c>
-      <c r="U2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="20"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1400,32 +1933,32 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1452,33 +1985,33 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>79</v>
+      <c r="A12" s="21" t="s">
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="21"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1503,32 +2036,32 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +2075,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44534BA-0940-439E-A6F0-9369F60D4010}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
minor change. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="104">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -182,22 +182,10 @@
     <t>S2325480HUID</t>
   </si>
   <si>
-    <t>EDBD19</t>
-  </si>
-  <si>
-    <t>201295</t>
-  </si>
-  <si>
     <t>S2021218GUID</t>
   </si>
   <si>
     <t>S2325481FUID</t>
-  </si>
-  <si>
-    <t>iWEALTH</t>
-  </si>
-  <si>
-    <t>SGMBONEAPPMB.ipa</t>
   </si>
   <si>
     <t>S2325482DUID</t>
@@ -295,9 +283,6 @@
     <t>APPLE_iPhone12mini_iOS_14.7.1_eaf14</t>
   </si>
   <si>
-    <t>APPLE_iPhone13Pro_iOS_15.2.0_2d8ea</t>
-  </si>
-  <si>
     <t>APPLE_iPhone11Pro_iOS_14.4.0_6ccce</t>
   </si>
   <si>
@@ -343,18 +328,6 @@
     <t>r36d4py9mtkykt29c925c7mg</t>
   </si>
   <si>
-    <t>APPLE_iPhone11Pro_iOS_13.0.0_3f7e0</t>
-  </si>
-  <si>
-    <t>13.0.0</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone12_iOS_14.1.0_a050d</t>
-  </si>
-  <si>
-    <t>14.1.0</t>
-  </si>
-  <si>
     <t>APPLE_iPhoneSE_iOS_14.6.0_9d61f</t>
   </si>
   <si>
@@ -370,9 +343,6 @@
     <t>15.0.0</t>
   </si>
   <si>
-    <t>APPLE_iPhone13Pro_iOS_15.0.0_2d2ae</t>
-  </si>
-  <si>
     <t>APPLE_iPhone8_iOS_14.0.1_aa631</t>
   </si>
   <si>
@@ -389,13 +359,16 @@
   </si>
   <si>
     <t>dbs_android_UAT_7_10_003_532.apk</t>
+  </si>
+  <si>
+    <t>SGMB_ONEAPP_MB-12-3-42.ipa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,12 +416,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF242424"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -477,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,16 +491,14 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -960,8 +925,8 @@
       <c r="N2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="22" t="s">
-        <v>112</v>
+      <c r="O2" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>22</v>
@@ -1005,13 +970,13 @@
         <v>5</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>22</v>
@@ -1025,158 +990,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="14" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>84</v>
+      <c r="H1" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>92</v>
       </c>
       <c r="K1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>103</v>
-      </c>
       <c r="P1" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="R1" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>98</v>
+      <c r="K2" t="s">
+        <v>82</v>
       </c>
       <c r="L2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>105</v>
-      </c>
-      <c r="R2" t="s">
-        <v>111</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1225,28 +1157,13 @@
       <c r="P3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -1276,37 +1193,22 @@
         <v>48</v>
       </c>
       <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" t="s">
         <v>52</v>
       </c>
-      <c r="M4" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="18" t="s">
-        <v>49</v>
+      <c r="O4" t="s">
+        <v>53</v>
       </c>
       <c r="P4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S4" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4" t="s">
-        <v>75</v>
-      </c>
-      <c r="U4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1349,29 +1251,14 @@
       <c r="N5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="19" t="s">
-        <v>50</v>
+      <c r="O5" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1420,23 +1307,8 @@
       <c r="P6" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1485,23 +1357,8 @@
       <c r="P7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1550,23 +1407,8 @@
       <c r="P8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1580,25 +1422,25 @@
         <v>3</v>
       </c>
       <c r="E9" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="11">
         <v>1</v>
       </c>
       <c r="G9" s="11">
+        <v>5</v>
+      </c>
+      <c r="H9" s="11">
         <v>1</v>
-      </c>
-      <c r="H9" s="11">
-        <v>5</v>
       </c>
       <c r="I9" s="11">
         <v>1</v>
       </c>
       <c r="J9" s="11">
+        <v>5</v>
+      </c>
+      <c r="K9" s="11">
         <v>1</v>
-      </c>
-      <c r="K9" s="11">
-        <v>5</v>
       </c>
       <c r="L9" s="11">
         <v>1</v>
@@ -1615,23 +1457,8 @@
       <c r="P9" s="11">
         <v>1</v>
       </c>
-      <c r="Q9" s="11">
-        <v>1</v>
-      </c>
-      <c r="R9" s="11">
-        <v>1</v>
-      </c>
-      <c r="S9" s="11">
-        <v>5</v>
-      </c>
-      <c r="T9" s="11">
-        <v>1</v>
-      </c>
-      <c r="U9" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1675,34 +1502,18 @@
         <v>37</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
@@ -1713,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:F13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,11 +1615,11 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>64</v>
+      <c r="A2" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
@@ -1838,38 +1649,38 @@
         <v>48</v>
       </c>
       <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
         <v>52</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>57</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>59</v>
       </c>
-      <c r="R2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1933,32 +1744,32 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1985,33 +1796,33 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F12" t="s">
         <v>72</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>73</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H12" t="s">
         <v>74</v>
       </c>
-      <c r="E12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -2036,32 +1847,32 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Data Modification Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="86">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -277,98 +277,44 @@
     <t>M4520239IUID</t>
   </si>
   <si>
-    <t>APPLE_iPhoneX_iOS_13.5.1_5640f</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone12mini_iOS_14.7.1_eaf14</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone11Pro_iOS_14.4.0_6ccce</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone11ProMax_iOS_14.4.2_de1da</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone12Pro_iOS_14.2.1_0d955</t>
-  </si>
-  <si>
-    <t>13.5.1</t>
-  </si>
-  <si>
-    <t>14.7.1</t>
-  </si>
-  <si>
-    <t>15.2.0</t>
-  </si>
-  <si>
-    <t>14.4.0</t>
-  </si>
-  <si>
-    <t>14.4.2</t>
-  </si>
-  <si>
-    <t>14.2.1</t>
-  </si>
-  <si>
-    <t>APPLE_iPhoneSE2020_iOS_13.6.1_4989f</t>
-  </si>
-  <si>
-    <t>APPLE_iPhoneXR_iOS_13.3.1_1cb9d</t>
-  </si>
-  <si>
-    <t>13.6.1</t>
-  </si>
-  <si>
-    <t>13.3.1</t>
-  </si>
-  <si>
     <t>divya.devi@crestechsoftware.com</t>
   </si>
   <si>
     <t>r36d4py9mtkykt29c925c7mg</t>
   </si>
   <si>
-    <t>APPLE_iPhoneSE_iOS_14.6.0_9d61f</t>
-  </si>
-  <si>
-    <t>14.6.0</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone13mini_iOS_15.2.0_22426</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone13_iOS_15.0.0_ad341</t>
-  </si>
-  <si>
-    <t>15.0.0</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone8_iOS_14.0.1_aa631</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone12ProMax_iOS_14.6.0_de280</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone8plus_iOS_14.6.0_5cd33</t>
-  </si>
-  <si>
-    <t>APPLE_iPhone7_iOS_14.4.0_589b8</t>
-  </si>
-  <si>
-    <t>14.0.1</t>
-  </si>
-  <si>
     <t>dbs_android_UAT_7_10_003_532.apk</t>
   </si>
   <si>
     <t>SGMB_ONEAPP_MB-12-3-42.ipa</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyOnMax_Android_8.1.0_85564</t>
+  </si>
+  <si>
+    <t>MOTOROLA_MotoG5_Android_8.1.0_c3d6c</t>
+  </si>
+  <si>
+    <t>XIAOMI_Redmi6_Android_9.0.0_ed157</t>
+  </si>
+  <si>
+    <t>XIAOMI_RedmiNote7Pro_Android_9.0.0_059d9</t>
+  </si>
+  <si>
+    <t>XIAOMI_RedmiNote9_Android_10.0.0_a7454</t>
+  </si>
+  <si>
+    <t>8.1.0</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,12 +345,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF202124"/>
       <name val="Arial"/>
@@ -431,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -439,12 +379,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -480,18 +450,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,6 +461,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -807,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,8 +893,8 @@
       <c r="N2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="18" t="s">
-        <v>102</v>
+      <c r="O2" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>22</v>
@@ -970,13 +938,13 @@
         <v>5</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>22</v>
@@ -990,175 +958,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" t="s">
-        <v>101</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1177,38 +1052,8 @@
       <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1227,38 +1072,8 @@
       <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1277,38 +1092,8 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1327,38 +1112,8 @@
       <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1377,38 +1132,8 @@
       <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1422,43 +1147,13 @@
         <v>3</v>
       </c>
       <c r="E9" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="11">
-        <v>1</v>
-      </c>
-      <c r="G9" s="11">
-        <v>5</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1</v>
-      </c>
-      <c r="I9" s="11">
-        <v>1</v>
-      </c>
-      <c r="J9" s="11">
-        <v>5</v>
-      </c>
-      <c r="K9" s="11">
-        <v>1</v>
-      </c>
-      <c r="L9" s="11">
-        <v>1</v>
-      </c>
-      <c r="M9" s="11">
-        <v>1</v>
-      </c>
-      <c r="N9" s="11">
-        <v>5</v>
-      </c>
-      <c r="O9" s="11">
-        <v>1</v>
-      </c>
-      <c r="P9" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1477,43 +1172,13 @@
       <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
@@ -1522,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P3"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1280,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B2" t="s">
@@ -1680,7 +1345,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="15"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1743,7 +1408,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1796,7 +1461,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B12" t="s">
@@ -1822,7 +1487,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="16"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1846,7 +1511,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1873,6 +1538,32 @@
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
main ios branch Signed-off-by: ShafqatLetCode <shafqat.ali@indianexpress.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -106,13 +106,13 @@
     <t>Device</t>
   </si>
   <si>
-    <t>Galaxy A12</t>
+    <t>iPhone 13</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>10.0.0</t>
+    <t>15.0.0</t>
   </si>
   <si>
     <t>OperatingSystem</t>
@@ -130,7 +130,7 @@
     <t>Manafacturer</t>
   </si>
   <si>
-    <t>Samsung</t>
+    <t>ios</t>
   </si>
   <si>
     <t>Min_Ver</t>
@@ -468,13 +468,13 @@
     <t>OPPO_A53_Android_10.0.0_bd07c</t>
   </si>
   <si>
-    <t>iPhone 13</t>
-  </si>
-  <si>
-    <t>15.0.0</t>
-  </si>
-  <si>
-    <t>ios</t>
+    <t>Galaxy A12</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -482,9 +482,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -531,14 +531,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -546,6 +539,36 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,63 +583,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -646,7 +616,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,13 +665,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -681,12 +681,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -699,19 +795,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,55 +813,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,79 +855,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,16 +921,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -952,24 +967,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -983,21 +985,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1007,31 +994,44 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1039,127 +1039,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1770,7 +1770,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.1428571428571" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1799,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2238,7 +2238,7 @@
   <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:A75"/>
+      <selection activeCell="B66" sqref="B66:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -2574,18 +2574,18 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2614,10 +2614,10 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:2">

</xml_diff>

<commit_message>
mailer added ios Signed-off-by: ShafqatLetCode <shafqat.ali@indianexpress.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -106,13 +106,13 @@
     <t>Device</t>
   </si>
   <si>
-    <t>iPhone 13</t>
+    <t>Galaxy A12</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>15.0.0</t>
+    <t>10.0.0</t>
   </si>
   <si>
     <t>OperatingSystem</t>
@@ -130,7 +130,7 @@
     <t>Manafacturer</t>
   </si>
   <si>
-    <t>ios</t>
+    <t>Samsung</t>
   </si>
   <si>
     <t>Min_Ver</t>
@@ -468,13 +468,13 @@
     <t>OPPO_A53_Android_10.0.0_bd07c</t>
   </si>
   <si>
-    <t>Galaxy A12</t>
-  </si>
-  <si>
-    <t>10.0.0</t>
-  </si>
-  <si>
-    <t>Samsung</t>
+    <t>iPhone 13</t>
+  </si>
+  <si>
+    <t>15.0.0</t>
+  </si>
+  <si>
+    <t>ios</t>
   </si>
 </sst>
 </file>
@@ -482,9 +482,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -530,8 +530,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,7 +553,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -559,6 +590,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -566,27 +612,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -614,24 +643,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -645,22 +658,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -681,13 +681,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,169 +861,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,17 +935,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -967,20 +961,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1011,16 +1009,21 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1029,9 +1032,6 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1039,127 +1039,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1770,7 +1770,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.1428571428571" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1799,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2238,7 +2238,7 @@
   <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B75"/>
+      <selection activeCell="A66" sqref="A66:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -2574,18 +2574,18 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2614,10 +2614,10 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:2">

</xml_diff>